<commit_message>
Calibração da Evapotranspiração no SMAP
Por meio de um coeficiente Ecof = 1.4, a evapotranspiração foi ajustada de modo a calibrar o modelo
</commit_message>
<xml_diff>
--- a/Applications/case.xlsx
+++ b/Applications/case.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\MOGESTpy\Applications\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="29280" yWindow="495" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
-    <sheet name="Params" sheetId="1" r:id="rId1"/>
+    <sheet name="Params" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,8 +75,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +88,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -230,7 +234,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -424,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,17 +436,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -922,7 +922,10 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>